<commit_message>
Added the title feature.
</commit_message>
<xml_diff>
--- a/samplePythonCode/TDWG databases.xlsx
+++ b/samplePythonCode/TDWG databases.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <s:bookViews>
     <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TDWG databases (3)" sheetId="1" r:id="rId1"/>
+    <s:sheet name="TDWG databases (3)" sheetId="1" r:id="rId1"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -559,7 +559,6 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -856,653 +855,653 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <cols>
-    <col style="1" width="9.1" customWidth="1" max="1" min="1"/>
-    <col style="1" width="9.1" customWidth="1" max="2" min="2"/>
-    <col style="1" width="9.1" customWidth="1" max="3" min="3"/>
-    <col style="1" width="9.1" customWidth="1" max="6" min="6"/>
+    <col customWidth="1" max="1" width="9.1" style="0" min="1"/>
+    <col customWidth="1" max="2" width="9.1" style="0" min="2"/>
+    <col customWidth="1" max="3" width="9.1" style="0" min="3"/>
+    <col customWidth="1" max="6" width="9.1" style="0" min="6"/>
   </cols>
   <sheetData>
-    <row spans="1:6" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
         <v>101</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>103</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row spans="1:6" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>138</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row spans="1:6" r="3">
-      <c t="s" r="A3">
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>139</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row spans="1:6" r="4">
-      <c t="s" r="A4">
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="1" r="B4">
+      <c r="B4" s="0" t="s">
         <v>125</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row spans="1:6" r="5">
-      <c t="s" r="A5">
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>137</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:6" r="6">
-      <c t="s" r="A6">
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>117</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:6" r="7">
-      <c t="s" r="A7">
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>140</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:6" r="8">
-      <c t="s" r="A8">
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>116</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row spans="1:6" r="9">
-      <c t="s" r="A9">
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>163</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row spans="1:6" r="10">
-      <c t="s" r="A10">
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>133</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row spans="1:6" r="11">
-      <c t="s" r="A11">
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="1" r="B11">
+      <c r="B11" s="0" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row spans="1:6" r="12">
-      <c t="s" r="A12">
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>142</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row spans="1:6" r="13">
-      <c t="s" r="A13">
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="B13">
+      <c r="B13" t="s">
         <v>134</v>
       </c>
-      <c t="s" r="C13">
+      <c r="C13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row spans="1:6" r="14">
-      <c t="s" r="A14">
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="B14">
+      <c r="B14" t="s">
         <v>143</v>
       </c>
-      <c t="s" r="C14">
+      <c r="C14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row spans="1:6" r="15">
-      <c t="s" r="A15">
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="B15">
+      <c r="B15" t="s">
         <v>114</v>
       </c>
-      <c t="s" r="C15">
+      <c r="C15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row spans="1:6" r="16">
-      <c t="s" r="A16">
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c t="s" r="B16">
+      <c r="B16" t="s">
         <v>159</v>
       </c>
-      <c t="s" r="C16">
+      <c r="C16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row spans="1:6" r="17">
-      <c t="s" r="A17">
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c t="s" r="B17">
+      <c r="B17" t="s">
         <v>119</v>
       </c>
-      <c t="s" r="C17">
+      <c r="C17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row spans="1:6" r="18">
-      <c t="s" r="A18">
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="B18">
+      <c r="B18" t="s">
         <v>136</v>
       </c>
-      <c t="s" r="C18">
+      <c r="C18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row spans="1:6" r="19">
-      <c t="s" r="A19">
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c t="s" r="B19">
+      <c r="B19" t="s">
         <v>145</v>
       </c>
-      <c t="s" r="C19">
+      <c r="C19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row spans="1:6" r="20">
-      <c t="s" r="A20">
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="B20">
+      <c r="B20" t="s">
         <v>115</v>
       </c>
-      <c t="s" r="C20">
+      <c r="C20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row spans="1:6" r="21">
-      <c t="s" r="A21">
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="B21">
+      <c r="B21" t="s">
         <v>147</v>
       </c>
-      <c t="s" r="C21">
+      <c r="C21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row spans="1:6" r="22">
-      <c t="s" r="A22">
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="B22">
+      <c r="B22" t="s">
         <v>118</v>
       </c>
-      <c t="s" r="C22">
+      <c r="C22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row spans="1:6" r="23">
-      <c t="s" r="A23">
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c t="s" r="B23">
+      <c r="B23" t="s">
         <v>149</v>
       </c>
-      <c t="s" r="C23">
+      <c r="C23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row spans="1:6" r="24">
-      <c t="s" r="A24">
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c t="s" r="B24">
+      <c r="B24" t="s">
         <v>148</v>
       </c>
-      <c t="s" r="C24">
+      <c r="C24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row spans="1:6" r="25">
-      <c t="s" r="A25">
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
         <v>41</v>
       </c>
-      <c t="s" r="B25">
+      <c r="B25" t="s">
         <v>150</v>
       </c>
-      <c t="s" r="C25">
+      <c r="C25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row spans="1:6" r="26">
-      <c t="s" r="A26">
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
         <v>42</v>
       </c>
-      <c t="s" r="B26">
+      <c r="B26" t="s">
         <v>161</v>
       </c>
-      <c t="s" r="C26">
+      <c r="C26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row spans="1:6" r="27">
-      <c t="s" r="A27">
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
         <v>45</v>
       </c>
-      <c t="s" r="B27">
+      <c r="B27" t="s">
         <v>131</v>
       </c>
-      <c t="s" r="C27">
+      <c r="C27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row spans="1:6" r="28">
-      <c t="s" r="A28">
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
         <v>46</v>
       </c>
-      <c t="s" r="B28">
+      <c r="B28" t="s">
         <v>126</v>
       </c>
-      <c t="s" r="C28">
+      <c r="C28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row spans="1:6" r="29">
-      <c t="s" r="A29">
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
         <v>47</v>
       </c>
-      <c t="s" r="B29">
+      <c r="B29" t="s">
         <v>123</v>
       </c>
-      <c t="s" r="C29">
+      <c r="C29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row spans="1:6" r="30">
-      <c t="s" r="A30">
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
         <v>48</v>
       </c>
-      <c t="s" r="B30">
+      <c r="B30" t="s">
         <v>154</v>
       </c>
-      <c t="s" r="C30">
+      <c r="C30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row spans="1:6" r="31">
-      <c t="s" r="A31">
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
         <v>49</v>
       </c>
-      <c t="s" r="B31">
+      <c r="B31" t="s">
         <v>124</v>
       </c>
-      <c t="s" r="C31">
+      <c r="C31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row spans="1:6" r="32">
-      <c t="s" r="A32">
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
         <v>50</v>
       </c>
-      <c t="s" r="B32">
+      <c r="B32" t="s">
         <v>151</v>
       </c>
-      <c t="s" r="C32">
+      <c r="C32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row spans="1:6" r="33">
-      <c t="s" r="A33">
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c t="s" r="B33">
+      <c r="B33" t="s">
         <v>153</v>
       </c>
-      <c t="s" r="C33">
+      <c r="C33" t="s">
         <v>98</v>
       </c>
     </row>
-    <row spans="1:6" r="34">
-      <c t="s" r="A34">
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
         <v>52</v>
       </c>
-      <c t="s" r="B34">
+      <c r="B34" t="s">
         <v>129</v>
       </c>
-      <c t="s" r="C34">
+      <c r="C34" t="s">
         <v>93</v>
       </c>
     </row>
-    <row spans="1:6" r="35">
-      <c t="s" r="A35">
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
         <v>59</v>
       </c>
-      <c t="s" r="B35">
+      <c r="B35" t="s">
         <v>130</v>
       </c>
-      <c t="s" r="C35">
+      <c r="C35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row spans="1:6" r="36">
-      <c t="s" r="A36">
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="1" r="B36"/>
-      <c t="s" r="C36">
+      <c r="B36" s="0" t="s"/>
+      <c r="C36" t="s">
         <v>54</v>
       </c>
-      <c t="s" r="F36">
+      <c r="F36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row spans="1:6" r="37">
-      <c t="s" r="A37">
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
         <v>62</v>
       </c>
-      <c t="s" r="B37">
+      <c r="B37" t="s">
         <v>157</v>
       </c>
-      <c t="s" r="C37">
+      <c r="C37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row spans="1:6" r="38">
-      <c t="s" r="A38">
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
         <v>63</v>
       </c>
-      <c t="s" r="B38">
+      <c r="B38" t="s">
         <v>158</v>
       </c>
-      <c t="s" r="C38">
+      <c r="C38" t="s">
         <v>94</v>
       </c>
     </row>
-    <row spans="1:6" r="39">
-      <c t="s" r="A39">
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
         <v>64</v>
       </c>
-      <c t="s" r="B39">
+      <c r="B39" t="s">
         <v>155</v>
       </c>
-      <c t="s" r="C39">
+      <c r="C39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row spans="1:6" r="40">
-      <c t="s" r="A40">
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
         <v>65</v>
       </c>
-      <c t="s" r="B40">
+      <c r="B40" t="s">
         <v>127</v>
       </c>
-      <c t="s" r="C40">
+      <c r="C40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:6" r="41">
-      <c t="s" r="A41">
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
         <v>66</v>
       </c>
-      <c t="s" r="B41">
+      <c r="B41" t="s">
         <v>156</v>
       </c>
-      <c t="s" r="C41">
+      <c r="C41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row spans="1:6" r="42">
-      <c t="s" r="A42">
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="1" r="B42">
+      <c r="B42" s="0" t="s">
         <v>152</v>
       </c>
-      <c t="s" r="C42">
+      <c r="C42" t="s">
         <v>68</v>
       </c>
     </row>
-    <row spans="1:6" r="43">
-      <c t="s" r="A43">
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
         <v>70</v>
       </c>
-      <c t="s" r="B43">
+      <c r="B43" t="s">
         <v>135</v>
       </c>
-      <c t="s" r="C43">
+      <c r="C43" t="s">
         <v>58</v>
       </c>
     </row>
-    <row spans="1:6" r="44">
-      <c t="s" r="A44">
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
         <v>72</v>
       </c>
-      <c t="s" r="B44">
+      <c r="B44" t="s">
         <v>144</v>
       </c>
-      <c t="s" r="C44">
+      <c r="C44" t="s">
         <v>76</v>
       </c>
     </row>
-    <row spans="1:6" r="45">
-      <c t="s" r="A45">
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
         <v>82</v>
       </c>
-      <c t="s" r="B45">
+      <c r="B45" t="s">
         <v>160</v>
       </c>
-      <c t="s" r="C45">
+      <c r="C45" t="s">
         <v>55</v>
       </c>
     </row>
-    <row spans="1:6" r="46">
-      <c t="s" r="A46">
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
         <v>83</v>
       </c>
-      <c t="s" r="B46">
+      <c r="B46" t="s">
         <v>162</v>
       </c>
-      <c t="s" r="C46">
+      <c r="C46" t="s">
         <v>78</v>
       </c>
     </row>
-    <row spans="1:6" r="47">
-      <c t="s" r="A47">
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
         <v>84</v>
       </c>
-      <c t="s" r="B47">
+      <c r="B47" t="s">
         <v>146</v>
       </c>
-      <c t="s" r="C47">
+      <c r="C47" t="s">
         <v>29</v>
       </c>
     </row>
-    <row spans="1:6" r="48">
-      <c t="s" r="A48">
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c t="s" r="B48">
+      <c r="B48" t="s">
         <v>164</v>
       </c>
-      <c t="s" r="C48">
+      <c r="C48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row spans="1:6" r="49">
-      <c t="s" r="A49">
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
         <v>97</v>
       </c>
-      <c t="s" r="B49">
+      <c r="B49" t="s">
         <v>132</v>
       </c>
-      <c t="s" r="C49">
+      <c r="C49" t="s">
         <v>35</v>
       </c>
     </row>
-    <row spans="1:6" r="50">
-      <c t="s" r="A50">
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="1" r="B50">
+      <c r="B50" s="0" t="s">
         <v>166</v>
       </c>
-      <c t="s" r="C50">
+      <c r="C50" t="s">
         <v>105</v>
       </c>
     </row>
-    <row spans="1:6" r="51">
-      <c t="s" r="A51">
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
         <v>104</v>
       </c>
-      <c t="s" r="B51">
+      <c r="B51" t="s">
         <v>165</v>
       </c>
-      <c t="s" r="C51">
+      <c r="C51" t="s">
         <v>106</v>
       </c>
     </row>
-    <row spans="1:6" r="52">
-      <c t="s" r="A52">
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
         <v>107</v>
       </c>
-      <c t="s" s="1" r="B52">
+      <c r="B52" s="0" t="s">
         <v>167</v>
       </c>
-      <c t="s" r="C52">
+      <c r="C52" t="s">
         <v>96</v>
       </c>
     </row>
-    <row spans="1:6" r="53">
-      <c t="s" r="A53">
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
         <v>108</v>
       </c>
-      <c t="s" r="B53">
+      <c r="B53" t="s">
         <v>121</v>
       </c>
-      <c t="s" r="C53">
+      <c r="C53" t="s">
         <v>57</v>
       </c>
     </row>
-    <row spans="1:6" r="54">
-      <c t="s" r="A54">
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
         <v>109</v>
       </c>
-      <c t="s" r="B54">
+      <c r="B54" t="s">
         <v>122</v>
       </c>
-      <c t="s" r="C54">
+      <c r="C54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row spans="1:6" r="55">
-      <c t="s" r="A55">
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
         <v>110</v>
       </c>
-      <c t="s" r="B55">
+      <c r="B55" t="s">
         <v>120</v>
       </c>
-      <c t="s" r="C55">
+      <c r="C55" t="s">
         <v>99</v>
       </c>
     </row>
-    <row spans="1:6" r="56">
-      <c t="s" r="A56">
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
         <v>111</v>
       </c>
-      <c t="s" r="B56">
+      <c r="B56" t="s">
         <v>128</v>
       </c>
-      <c t="s" r="C56">
+      <c r="C56" t="s">
         <v>79</v>
       </c>
     </row>
-    <row spans="1:6" r="57">
-      <c t="s" r="A57">
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
         <v>113</v>
       </c>
-      <c t="s" r="B57">
+      <c r="B57" t="s">
         <v>168</v>
       </c>
-      <c t="s" r="C57">
+      <c r="C57" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageMargins right="0.75" footer="0.5" left="0.75" top="1" bottom="1" header="0.5"/>
 </worksheet>
 </file>
</xml_diff>